<commit_message>
Updated analysis dated 11/15/2022 Updated Stata-to-R file structure and associated readme file. Fixed miscalculation in biomass-weighted body size Fixed errors in commonness calculations
</commit_message>
<xml_diff>
--- a/output/20221109/tables/betas_traits.xlsx
+++ b/output/20221109/tables/betas_traits.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,17 +10,17 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC711F7F-21FA-2F4E-B13A-525D0B8FE12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500"/>
   </bookViews>
   <sheets>
     <sheet name="traits models" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="26">
   <si>
     <t>Outcome</t>
   </si>
@@ -142,9 +142,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,17 +461,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="D30" sqref="D30:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="6" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +500,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -529,7 +529,7 @@
         <v>0.52366214990615845</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -558,7 +558,7 @@
         <v>0.52366214990615845</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -587,7 +587,7 @@
         <v>0.50216466188430786</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -610,13 +610,13 @@
         <v>23</v>
       </c>
       <c r="H5" s="1">
-        <v>8.3859793841838837E-2</v>
+        <v>0.083859793841838837</v>
       </c>
       <c r="I5" s="1">
         <v>0.49338066577911377</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -630,7 +630,7 @@
         <v>0.83416163921356201</v>
       </c>
       <c r="E6" s="1">
-        <v>3.5358820110559464E-2</v>
+        <v>0.035358820110559464</v>
       </c>
       <c r="F6" t="s">
         <v>1</v>
@@ -645,7 +645,7 @@
         <v>0.9034649133682251</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -659,7 +659,7 @@
         <v>0.82761919498443604</v>
       </c>
       <c r="E7" s="1">
-        <v>3.5672932863235474E-2</v>
+        <v>0.035672932863235474</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
@@ -674,7 +674,7 @@
         <v>0.89753812551498413</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -688,7 +688,7 @@
         <v>0.82396471500396729</v>
       </c>
       <c r="E8" s="1">
-        <v>3.5472676157951355E-2</v>
+        <v>0.035472676157951355</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
@@ -703,7 +703,7 @@
         <v>0.89349114894866943</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -717,7 +717,7 @@
         <v>0.82932811975479126</v>
       </c>
       <c r="E9" s="1">
-        <v>3.352968767285347E-2</v>
+        <v>0.03352968767285347</v>
       </c>
       <c r="F9" t="s">
         <v>1</v>
@@ -732,7 +732,7 @@
         <v>0.89504629373550415</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -761,7 +761,7 @@
         <v>1.1147490739822388</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -784,13 +784,13 @@
         <v>23</v>
       </c>
       <c r="H11" s="1">
-        <v>8.3164937794208527E-2</v>
+        <v>0.083164937794208527</v>
       </c>
       <c r="I11" s="1">
         <v>0.95710194110870361</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -819,7 +819,7 @@
         <v>0.92468816041946411</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -848,7 +848,7 @@
         <v>0.951973557472229</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -871,13 +871,13 @@
         <v>23</v>
       </c>
       <c r="H14" s="1">
-        <v>6.0346517711877823E-2</v>
+        <v>0.060346517711877823</v>
       </c>
       <c r="I14" s="1">
         <v>0.47596254944801331</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -900,13 +900,13 @@
         <v>23</v>
       </c>
       <c r="H15" s="1">
-        <v>9.0785764157772064E-2</v>
+        <v>0.090785764157772064</v>
       </c>
       <c r="I15" s="1">
         <v>0.513588547706604</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -929,13 +929,13 @@
         <v>23</v>
       </c>
       <c r="H16" s="1">
-        <v>6.515975296497345E-2</v>
+        <v>0.06515975296497345</v>
       </c>
       <c r="I16" s="1">
         <v>0.49540045857429504</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -958,13 +958,13 @@
         <v>23</v>
       </c>
       <c r="H17" s="1">
-        <v>6.0741964727640152E-2</v>
+        <v>0.060741964727640152</v>
       </c>
       <c r="I17" s="1">
         <v>0.49687516689300537</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -975,7 +975,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="1">
-        <v>-9.656853973865509E-2</v>
+        <v>-0.09656853973865509</v>
       </c>
       <c r="E18" s="1">
         <v>0.18529711663722992</v>
@@ -993,7 +993,7 @@
         <v>0.26661381125450134</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>0.57752424478530884</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>0.57059204578399658</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>0.62982988357543945</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1091,10 +1091,10 @@
         <v>15</v>
       </c>
       <c r="D22" s="1">
-        <v>6.4980745315551758E-2</v>
+        <v>0.14027746021747589</v>
       </c>
       <c r="E22" s="1">
-        <v>4.2514748871326447E-2</v>
+        <v>0.11668840050697327</v>
       </c>
       <c r="F22" t="s">
         <v>12</v>
@@ -1103,13 +1103,13 @@
         <v>23</v>
       </c>
       <c r="H22" s="1">
-        <v>-1.8348162993788719E-2</v>
+        <v>-0.088431805372238159</v>
       </c>
       <c r="I22" s="1">
-        <v>0.14830964803695679</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.36898672580718994</v>
+      </c>
+    </row>
+    <row r="23" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1120,10 +1120,10 @@
         <v>16</v>
       </c>
       <c r="D23" s="1">
-        <v>7.0458464324474335E-2</v>
+        <v>0.14242148399353027</v>
       </c>
       <c r="E23" s="1">
-        <v>4.1666612029075623E-2</v>
+        <v>0.11730613559484482</v>
       </c>
       <c r="F23" t="s">
         <v>12</v>
@@ -1132,13 +1132,13 @@
         <v>23</v>
       </c>
       <c r="H23" s="1">
-        <v>-1.1208095587790012E-2</v>
+        <v>-0.087498538196086884</v>
       </c>
       <c r="I23" s="1">
-        <v>0.1521250307559967</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.37234151363372803</v>
+      </c>
+    </row>
+    <row r="24" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1149,10 +1149,10 @@
         <v>17</v>
       </c>
       <c r="D24" s="1">
-        <v>6.6939085721969604E-2</v>
+        <v>0.10795728862285614</v>
       </c>
       <c r="E24" s="1">
-        <v>3.9027232676744461E-2</v>
+        <v>0.11208325624465942</v>
       </c>
       <c r="F24" t="s">
         <v>12</v>
@@ -1161,13 +1161,13 @@
         <v>23</v>
       </c>
       <c r="H24" s="1">
-        <v>-9.5542902126908302E-3</v>
+        <v>-0.11172589659690857</v>
       </c>
       <c r="I24" s="1">
-        <v>0.14343246817588806</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.32764047384262085</v>
+      </c>
+    </row>
+    <row r="25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1178,10 +1178,10 @@
         <v>18</v>
       </c>
       <c r="D25" s="1">
-        <v>6.4519420266151428E-2</v>
+        <v>0.08884245902299881</v>
       </c>
       <c r="E25" s="1">
-        <v>3.7882275879383087E-2</v>
+        <v>0.10794274508953094</v>
       </c>
       <c r="F25" t="s">
         <v>12</v>
@@ -1190,13 +1190,13 @@
         <v>23</v>
       </c>
       <c r="H25" s="1">
-        <v>-9.7298407927155495E-3</v>
+        <v>-0.12272532284259796</v>
       </c>
       <c r="I25" s="1">
-        <v>0.13876868784427643</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.30041024088859558</v>
+      </c>
+    </row>
+    <row r="26" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1206,11 +1206,11 @@
       <c r="C26" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="2">
-        <v>0.25857686996459961</v>
-      </c>
-      <c r="E26" s="2">
-        <v>2.4502338841557503E-2</v>
+      <c r="D26" s="1">
+        <v>0.77207005023956299</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.042151398956775665</v>
       </c>
       <c r="F26" t="s">
         <v>4</v>
@@ -1219,13 +1219,13 @@
         <v>23</v>
       </c>
       <c r="H26" s="1">
-        <v>0.21055229008197784</v>
+        <v>0.68945330381393433</v>
       </c>
       <c r="I26" s="1">
-        <v>0.30660146474838257</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.85468679666519165</v>
+      </c>
+    </row>
+    <row r="27" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1236,10 +1236,10 @@
         <v>16</v>
       </c>
       <c r="D27" s="1">
-        <v>0.25838309526443481</v>
+        <v>0.76948380470275879</v>
       </c>
       <c r="E27" s="1">
-        <v>2.6019487529993057E-2</v>
+        <v>0.041588019579648972</v>
       </c>
       <c r="F27" t="s">
         <v>4</v>
@@ -1248,13 +1248,13 @@
         <v>23</v>
       </c>
       <c r="H27" s="1">
-        <v>0.20738489925861359</v>
+        <v>0.68797129392623901</v>
       </c>
       <c r="I27" s="1">
-        <v>0.30938127636909485</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.85099631547927856</v>
+      </c>
+    </row>
+    <row r="28" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1265,10 +1265,10 @@
         <v>17</v>
       </c>
       <c r="D28" s="1">
-        <v>0.25672644376754761</v>
+        <v>0.76129913330078125</v>
       </c>
       <c r="E28" s="1">
-        <v>2.6141410693526268E-2</v>
+        <v>0.041200410574674606</v>
       </c>
       <c r="F28" t="s">
         <v>4</v>
@@ -1277,13 +1277,13 @@
         <v>23</v>
       </c>
       <c r="H28" s="1">
-        <v>0.20548927783966064</v>
+        <v>0.6805463433265686</v>
       </c>
       <c r="I28" s="1">
-        <v>0.30796360969543457</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.8420519232749939</v>
+      </c>
+    </row>
+    <row r="29" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1294,10 +1294,10 @@
         <v>18</v>
       </c>
       <c r="D29" s="1">
-        <v>0.25890171527862549</v>
+        <v>0.77160775661468506</v>
       </c>
       <c r="E29" s="1">
-        <v>2.5020383298397064E-2</v>
+        <v>0.0373099185526371</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
@@ -1306,13 +1306,13 @@
         <v>23</v>
       </c>
       <c r="H29" s="1">
-        <v>0.20986177027225494</v>
+        <v>0.69848030805587769</v>
       </c>
       <c r="I29" s="1">
-        <v>0.30794167518615723</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.84473520517349243</v>
+      </c>
+    </row>
+    <row r="30" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1322,11 +1322,11 @@
       <c r="C30" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="3">
-        <v>5.1090078353881836</v>
+      <c r="D30" s="1">
+        <v>1.0425946712493896</v>
       </c>
       <c r="E30" s="1">
-        <v>0.47292757034301758</v>
+        <v>0.11899025738239288</v>
       </c>
       <c r="F30" t="s">
         <v>4</v>
@@ -1335,13 +1335,13 @@
         <v>23</v>
       </c>
       <c r="H30" s="1">
-        <v>4.1820697784423828</v>
+        <v>0.80937379598617554</v>
       </c>
       <c r="I30" s="1">
-        <v>6.0359458923339844</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.2758156061172485</v>
+      </c>
+    </row>
+    <row r="31" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1351,11 +1351,11 @@
       <c r="C31" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="3">
-        <v>5.0843930244445801</v>
+      <c r="D31" s="1">
+        <v>1.0748137235641479</v>
       </c>
       <c r="E31" s="1">
-        <v>0.47662451863288879</v>
+        <v>0.1058812290430069</v>
       </c>
       <c r="F31" t="s">
         <v>4</v>
@@ -1364,13 +1364,13 @@
         <v>23</v>
       </c>
       <c r="H31" s="1">
-        <v>4.1502089500427246</v>
+        <v>0.86728650331497192</v>
       </c>
       <c r="I31" s="1">
-        <v>6.0185770988464355</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.2823408842086792</v>
+      </c>
+    </row>
+    <row r="32" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1380,11 +1380,11 @@
       <c r="C32" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="3">
-        <v>5.1003851890563965</v>
+      <c r="D32" s="1">
+        <v>1.0728994607925415</v>
       </c>
       <c r="E32" s="1">
-        <v>0.48571106791496277</v>
+        <v>0.10561241954565048</v>
       </c>
       <c r="F32" t="s">
         <v>4</v>
@@ -1393,13 +1393,13 @@
         <v>23</v>
       </c>
       <c r="H32" s="1">
-        <v>4.1483917236328125</v>
+        <v>0.86589914560317993</v>
       </c>
       <c r="I32" s="1">
-        <v>6.0523786544799805</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.2798998355865479</v>
+      </c>
+    </row>
+    <row r="33" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1409,11 +1409,11 @@
       <c r="C33" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="3">
-        <v>5.0693788528442383</v>
+      <c r="D33" s="1">
+        <v>1.0615861415863037</v>
       </c>
       <c r="E33" s="1">
-        <v>0.46401277184486389</v>
+        <v>0.099985666573047638</v>
       </c>
       <c r="F33" t="s">
         <v>4</v>
@@ -1422,13 +1422,13 @@
         <v>23</v>
       </c>
       <c r="H33" s="1">
-        <v>4.1599140167236328</v>
+        <v>0.86561423540115356</v>
       </c>
       <c r="I33" s="1">
-        <v>5.9788436889648438</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1.2575581073760986</v>
+      </c>
+    </row>
+    <row r="34" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1439,10 +1439,10 @@
         <v>15</v>
       </c>
       <c r="D34" s="1">
-        <v>1.7295666038990021E-2</v>
+        <v>0.13906879723072052</v>
       </c>
       <c r="E34" s="1">
-        <v>1.2832265347242355E-2</v>
+        <v>0.094747200608253479</v>
       </c>
       <c r="F34" t="s">
         <v>12</v>
@@ -1451,13 +1451,13 @@
         <v>23</v>
       </c>
       <c r="H34" s="1">
-        <v>-7.8555736690759659E-3</v>
+        <v>-0.046635717153549194</v>
       </c>
       <c r="I34" s="1">
-        <v>4.2446907609701157E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.32477331161499023</v>
+      </c>
+    </row>
+    <row r="35" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1468,10 +1468,10 @@
         <v>16</v>
       </c>
       <c r="D35" s="1">
-        <v>1.8728595227003098E-2</v>
+        <v>0.14309486746788025</v>
       </c>
       <c r="E35" s="1">
-        <v>1.3068582862615585E-2</v>
+        <v>0.094752080738544464</v>
       </c>
       <c r="F35" t="s">
         <v>12</v>
@@ -1480,13 +1480,13 @@
         <v>23</v>
       </c>
       <c r="H35" s="1">
-        <v>-6.8858270533382893E-3</v>
+        <v>-0.042619209736585617</v>
       </c>
       <c r="I35" s="1">
-        <v>4.4343017041683197E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.32880893349647522</v>
+      </c>
+    </row>
+    <row r="36" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1497,10 +1497,10 @@
         <v>17</v>
       </c>
       <c r="D36" s="1">
-        <v>1.6656547784805298E-2</v>
+        <v>0.11057703197002411</v>
       </c>
       <c r="E36" s="1">
-        <v>1.2908989563584328E-2</v>
+        <v>0.087860293686389923</v>
       </c>
       <c r="F36" t="s">
         <v>12</v>
@@ -1509,13 +1509,13 @@
         <v>23</v>
       </c>
       <c r="H36" s="1">
-        <v>-8.6450716480612755E-3</v>
+        <v>-0.061629142612218857</v>
       </c>
       <c r="I36" s="1">
-        <v>4.1958168148994446E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.28278321027755737</v>
+      </c>
+    </row>
+    <row r="37" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1526,10 +1526,10 @@
         <v>18</v>
       </c>
       <c r="D37" s="1">
-        <v>1.6969116404652596E-2</v>
+        <v>0.11663152277469635</v>
       </c>
       <c r="E37" s="1">
-        <v>1.2862409465014935E-2</v>
+        <v>0.087988920509815216</v>
       </c>
       <c r="F37" t="s">
         <v>12</v>
@@ -1538,13 +1538,13 @@
         <v>23</v>
       </c>
       <c r="H37" s="1">
-        <v>-8.2412064075469971E-3</v>
+        <v>-0.055826760828495026</v>
       </c>
       <c r="I37" s="1">
-        <v>4.2179439216852188E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.28908979892730713</v>
+      </c>
+    </row>
+    <row r="38" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1555,10 +1555,10 @@
         <v>15</v>
       </c>
       <c r="D38" s="1">
-        <v>0.31161564588546753</v>
+        <v>0.26149716973304749</v>
       </c>
       <c r="E38" s="1">
-        <v>0.25150144100189209</v>
+        <v>0.17170630395412445</v>
       </c>
       <c r="F38" t="s">
         <v>12</v>
@@ -1567,13 +1567,13 @@
         <v>23</v>
       </c>
       <c r="H38" s="1">
-        <v>-0.18132717907428741</v>
+        <v>-0.075047187507152557</v>
       </c>
       <c r="I38" s="1">
-        <v>0.80455845594406128</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.59804153442382812</v>
+      </c>
+    </row>
+    <row r="39" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1584,10 +1584,10 @@
         <v>16</v>
       </c>
       <c r="D39" s="1">
-        <v>0.34132975339889526</v>
+        <v>0.23487716913223267</v>
       </c>
       <c r="E39" s="1">
-        <v>0.24897119402885437</v>
+        <v>0.17081649601459503</v>
       </c>
       <c r="F39" t="s">
         <v>12</v>
@@ -1596,13 +1596,13 @@
         <v>23</v>
       </c>
       <c r="H39" s="1">
-        <v>-0.14665378630161285</v>
+        <v>-0.099923163652420044</v>
       </c>
       <c r="I39" s="1">
-        <v>0.82931327819824219</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.56967747211456299</v>
+      </c>
+    </row>
+    <row r="40" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1613,10 +1613,10 @@
         <v>17</v>
       </c>
       <c r="D40" s="1">
-        <v>0.32072135806083679</v>
+        <v>0.1825009286403656</v>
       </c>
       <c r="E40" s="1">
-        <v>0.23748336732387543</v>
+        <v>0.17015379667282104</v>
       </c>
       <c r="F40" t="s">
         <v>12</v>
@@ -1625,13 +1625,13 @@
         <v>23</v>
       </c>
       <c r="H40" s="1">
-        <v>-0.14474603533744812</v>
+        <v>-0.15100051462650299</v>
       </c>
       <c r="I40" s="1">
-        <v>0.78618878126144409</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.516002357006073</v>
+      </c>
+    </row>
+    <row r="41" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1642,10 +1642,10 @@
         <v>18</v>
       </c>
       <c r="D41" s="1">
-        <v>0.29456716775894165</v>
+        <v>0.14255504310131073</v>
       </c>
       <c r="E41" s="1">
-        <v>0.22347712516784668</v>
+        <v>0.1631043553352356</v>
       </c>
       <c r="F41" t="s">
         <v>12</v>
@@ -1654,13 +1654,13 @@
         <v>23</v>
       </c>
       <c r="H41" s="1">
-        <v>-0.14344799518585205</v>
+        <v>-0.17712949216365814</v>
       </c>
       <c r="I41" s="1">
-        <v>0.73258233070373535</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.4622395932674408</v>
+      </c>
+    </row>
+    <row r="42" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -1671,10 +1671,10 @@
         <v>15</v>
       </c>
       <c r="D42" s="1">
-        <v>6.7957125604152679E-2</v>
+        <v>0.004408013541251421</v>
       </c>
       <c r="E42" s="1">
-        <v>2.4345852434635162E-2</v>
+        <v>0.0013329912908375263</v>
       </c>
       <c r="F42" t="s">
         <v>13</v>
@@ -1683,13 +1683,13 @@
         <v>23</v>
       </c>
       <c r="H42" s="1">
-        <v>2.0239254459738731E-2</v>
+        <v>0.0017953505739569664</v>
       </c>
       <c r="I42" s="1">
-        <v>0.11567499488592148</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.0070206765085458755</v>
+      </c>
+    </row>
+    <row r="43" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -1700,10 +1700,10 @@
         <v>16</v>
       </c>
       <c r="D43" s="1">
-        <v>7.6589316129684448E-2</v>
+        <v>0.0056173233315348625</v>
       </c>
       <c r="E43" s="1">
-        <v>2.379353903234005E-2</v>
+        <v>0.0010347436182200909</v>
       </c>
       <c r="F43" t="s">
         <v>13</v>
@@ -1712,13 +1712,13 @@
         <v>23</v>
       </c>
       <c r="H43" s="1">
-        <v>2.9953978955745697E-2</v>
+        <v>0.0035892259329557419</v>
       </c>
       <c r="I43" s="1">
-        <v>0.1232246533036232</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.0076454207301139832</v>
+      </c>
+    </row>
+    <row r="44" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1729,10 +1729,10 @@
         <v>17</v>
       </c>
       <c r="D44" s="1">
-        <v>7.2674103081226349E-2</v>
+        <v>0.0050881188362836838</v>
       </c>
       <c r="E44" s="1">
-        <v>2.342771552503109E-2</v>
+        <v>0.0011296549346297979</v>
       </c>
       <c r="F44" t="s">
         <v>13</v>
@@ -1741,13 +1741,13 @@
         <v>23</v>
       </c>
       <c r="H44" s="1">
-        <v>2.6755779981613159E-2</v>
+        <v>0.0028739951085299253</v>
       </c>
       <c r="I44" s="1">
-        <v>0.11859242618083954</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.0073022423312067986</v>
+      </c>
+    </row>
+    <row r="45" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -1758,10 +1758,10 @@
         <v>18</v>
       </c>
       <c r="D45" s="1">
-        <v>7.1386761963367462E-2</v>
+        <v>0.0049827666953206062</v>
       </c>
       <c r="E45" s="1">
-        <v>2.2708462551236153E-2</v>
+        <v>0.0010449381079524755</v>
       </c>
       <c r="F45" t="s">
         <v>13</v>
@@ -1770,13 +1770,13 @@
         <v>23</v>
       </c>
       <c r="H45" s="1">
-        <v>2.6878176257014275E-2</v>
+        <v>0.0029346880037337542</v>
       </c>
       <c r="I45" s="1">
-        <v>0.1158953458070755</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.007030845619738102</v>
+      </c>
+    </row>
+    <row r="46" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -1787,10 +1787,10 @@
         <v>15</v>
       </c>
       <c r="D46" s="1">
-        <v>0.29692757129669189</v>
+        <v>0.25779908895492554</v>
       </c>
       <c r="E46" s="1">
-        <v>4.4808514416217804E-2</v>
+        <v>0.041645646095275879</v>
       </c>
       <c r="F46" t="s">
         <v>7</v>
@@ -1799,13 +1799,13 @@
         <v>23</v>
       </c>
       <c r="H46" s="1">
-        <v>0.20910288393497467</v>
+        <v>0.1761736273765564</v>
       </c>
       <c r="I46" s="1">
-        <v>0.38475227355957031</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.33942455053329468</v>
+      </c>
+    </row>
+    <row r="47" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -1816,10 +1816,10 @@
         <v>16</v>
       </c>
       <c r="D47" s="1">
-        <v>0.30065038800239563</v>
+        <v>0.25800672173500061</v>
       </c>
       <c r="E47" s="1">
-        <v>4.755396768450737E-2</v>
+        <v>0.045938912779092789</v>
       </c>
       <c r="F47" t="s">
         <v>7</v>
@@ -1828,13 +1828,13 @@
         <v>23</v>
       </c>
       <c r="H47" s="1">
-        <v>0.20744460821151733</v>
+        <v>0.16796645522117615</v>
       </c>
       <c r="I47" s="1">
-        <v>0.39385616779327393</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.34804698824882507</v>
+      </c>
+    </row>
+    <row r="48" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -1845,10 +1845,10 @@
         <v>17</v>
       </c>
       <c r="D48" s="1">
-        <v>0.29944732785224915</v>
+        <v>0.25650396943092346</v>
       </c>
       <c r="E48" s="1">
-        <v>4.9361392855644226E-2</v>
+        <v>0.047062192112207413</v>
       </c>
       <c r="F48" t="s">
         <v>7</v>
@@ -1857,13 +1857,13 @@
         <v>23</v>
       </c>
       <c r="H48" s="1">
-        <v>0.20269899070262909</v>
+        <v>0.1642620712518692</v>
       </c>
       <c r="I48" s="1">
-        <v>0.39619565010070801</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.34874585270881653</v>
+      </c>
+    </row>
+    <row r="49" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -1874,10 +1874,10 @@
         <v>18</v>
       </c>
       <c r="D49" s="1">
-        <v>0.3005598783493042</v>
+        <v>0.2575933039188385</v>
       </c>
       <c r="E49" s="1">
-        <v>4.9118176102638245E-2</v>
+        <v>0.04659251868724823</v>
       </c>
       <c r="F49" t="s">
         <v>7</v>
@@ -1886,13 +1886,13 @@
         <v>23</v>
       </c>
       <c r="H49" s="1">
-        <v>0.20428825914859772</v>
+        <v>0.16627196967601776</v>
       </c>
       <c r="I49" s="1">
-        <v>0.39683151245117188</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.34891465306282043</v>
+      </c>
+    </row>
+    <row r="50" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -1903,10 +1903,10 @@
         <v>15</v>
       </c>
       <c r="D50" s="1">
-        <v>5.3888654708862305</v>
+        <v>5.0924191474914551</v>
       </c>
       <c r="E50" s="1">
-        <v>0.65780550241470337</v>
+        <v>0.57012712955474854</v>
       </c>
       <c r="F50" t="s">
         <v>7</v>
@@ -1915,13 +1915,13 @@
         <v>23</v>
       </c>
       <c r="H50" s="1">
-        <v>4.0995664596557617</v>
+        <v>3.9749698638916016</v>
       </c>
       <c r="I50" s="1">
-        <v>6.6781644821166992</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+        <v>6.2098684310913086</v>
+      </c>
+    </row>
+    <row r="51" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -1932,10 +1932,10 @@
         <v>16</v>
       </c>
       <c r="D51" s="1">
-        <v>5.3916444778442383</v>
+        <v>5.1469736099243164</v>
       </c>
       <c r="E51" s="1">
-        <v>0.67701417207717896</v>
+        <v>0.60361486673355103</v>
       </c>
       <c r="F51" t="s">
         <v>7</v>
@@ -1944,13 +1944,13 @@
         <v>23</v>
       </c>
       <c r="H51" s="1">
-        <v>4.0646967887878418</v>
+        <v>3.96388840675354</v>
       </c>
       <c r="I51" s="1">
-        <v>6.7185921669006348</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+        <v>6.3300585746765137</v>
+      </c>
+    </row>
+    <row r="52" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -1961,10 +1961,10 @@
         <v>17</v>
       </c>
       <c r="D52" s="1">
-        <v>5.4202699661254883</v>
+        <v>5.1798076629638672</v>
       </c>
       <c r="E52" s="1">
-        <v>0.70410233736038208</v>
+        <v>0.62599378824234009</v>
       </c>
       <c r="F52" t="s">
         <v>7</v>
@@ -1973,13 +1973,13 @@
         <v>23</v>
       </c>
       <c r="H52" s="1">
-        <v>4.040229320526123</v>
+        <v>3.9528598785400391</v>
       </c>
       <c r="I52" s="1">
-        <v>6.8003106117248535</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+        <v>6.4067554473876953</v>
+      </c>
+    </row>
+    <row r="53" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -1990,10 +1990,10 @@
         <v>18</v>
       </c>
       <c r="D53" s="1">
-        <v>5.4023027420043945</v>
+        <v>5.1506638526916504</v>
       </c>
       <c r="E53" s="1">
-        <v>0.69024932384490967</v>
+        <v>0.60268157720565796</v>
       </c>
       <c r="F53" t="s">
         <v>7</v>
@@ -2002,13 +2002,13 @@
         <v>23</v>
       </c>
       <c r="H53" s="1">
-        <v>4.0494141578674316</v>
+        <v>3.9694080352783203</v>
       </c>
       <c r="I53" s="1">
-        <v>6.7551913261413574</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+        <v>6.3319196701049805</v>
+      </c>
+    </row>
+    <row r="54" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2019,10 +2019,10 @@
         <v>15</v>
       </c>
       <c r="D54" s="1">
-        <v>2.2468969225883484E-2</v>
+        <v>0.0014742759522050619</v>
       </c>
       <c r="E54" s="1">
-        <v>1.0701911523938179E-2</v>
+        <v>0.00070770381717011333</v>
       </c>
       <c r="F54" t="s">
         <v>13</v>
@@ -2031,13 +2031,13 @@
         <v>23</v>
       </c>
       <c r="H54" s="1">
-        <v>1.4932226622477174E-3</v>
+        <v>8.7176471424754709e-05</v>
       </c>
       <c r="I54" s="1">
-        <v>4.3444715440273285E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.002861375454813242</v>
+      </c>
+    </row>
+    <row r="55" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -2048,10 +2048,10 @@
         <v>16</v>
       </c>
       <c r="D55" s="1">
-        <v>2.4643756449222565E-2</v>
+        <v>0.0017883059335872531</v>
       </c>
       <c r="E55" s="1">
-        <v>1.1264222674071789E-2</v>
+        <v>0.00086507474770769477</v>
       </c>
       <c r="F55" t="s">
         <v>13</v>
@@ -2060,13 +2060,13 @@
         <v>23</v>
       </c>
       <c r="H55" s="1">
-        <v>2.5658800732344389E-3</v>
+        <v>9.2759430117439479e-05</v>
       </c>
       <c r="I55" s="1">
-        <v>4.6721633523702621E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.0034838523715734482</v>
+      </c>
+    </row>
+    <row r="56" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -2077,10 +2077,10 @@
         <v>17</v>
       </c>
       <c r="D56" s="1">
-        <v>2.2793896496295929E-2</v>
+        <v>0.0015272855525836349</v>
       </c>
       <c r="E56" s="1">
-        <v>1.1189954355359077E-2</v>
+        <v>0.00080164504470303655</v>
       </c>
       <c r="F56" t="s">
         <v>13</v>
@@ -2089,13 +2089,13 @@
         <v>23</v>
       </c>
       <c r="H56" s="1">
-        <v>8.6158595513552427E-4</v>
+        <v>-4.3938736780546606e-05</v>
       </c>
       <c r="I56" s="1">
-        <v>4.4726207852363586E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.0030985097400844097</v>
+      </c>
+    </row>
+    <row r="57" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -2106,10 +2106,10 @@
         <v>18</v>
       </c>
       <c r="D57" s="1">
-        <v>2.2866927087306976E-2</v>
+        <v>0.0015238305786624551</v>
       </c>
       <c r="E57" s="1">
-        <v>1.0892243124544621E-2</v>
+        <v>0.00079698028275743127</v>
       </c>
       <c r="F57" t="s">
         <v>13</v>
@@ -2118,13 +2118,13 @@
         <v>23</v>
       </c>
       <c r="H57" s="1">
-        <v>1.5181305352598429E-3</v>
+        <v>-3.8250775105552748e-05</v>
       </c>
       <c r="I57" s="1">
-        <v>4.4215723872184753E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.0030859119724482298</v>
+      </c>
+    </row>
+    <row r="58" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>9</v>
       </c>
@@ -2135,10 +2135,10 @@
         <v>15</v>
       </c>
       <c r="D58" s="1">
-        <v>0.2934863269329071</v>
+        <v>0.013377105817198753</v>
       </c>
       <c r="E58" s="1">
-        <v>0.13513800501823425</v>
+        <v>0.0069817281328141689</v>
       </c>
       <c r="F58" t="s">
         <v>13</v>
@@ -2147,13 +2147,13 @@
         <v>23</v>
       </c>
       <c r="H58" s="1">
-        <v>2.8615837916731834E-2</v>
+        <v>-0.00030708132544532418</v>
       </c>
       <c r="I58" s="1">
-        <v>0.55835682153701782</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.02706129290163517</v>
+      </c>
+    </row>
+    <row r="59" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>9</v>
       </c>
@@ -2164,10 +2164,10 @@
         <v>16</v>
       </c>
       <c r="D59" s="1">
-        <v>0.33867403864860535</v>
+        <v>0.018711445853114128</v>
       </c>
       <c r="E59" s="1">
-        <v>0.1368652731180191</v>
+        <v>0.007450637873262167</v>
       </c>
       <c r="F59" t="s">
         <v>13</v>
@@ -2176,13 +2176,13 @@
         <v>23</v>
       </c>
       <c r="H59" s="1">
-        <v>7.0418104529380798E-2</v>
+        <v>0.0041081956587731838</v>
       </c>
       <c r="I59" s="1">
-        <v>0.6069299578666687</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.033314697444438934</v>
+      </c>
+    </row>
+    <row r="60" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>9</v>
       </c>
@@ -2193,10 +2193,10 @@
         <v>17</v>
       </c>
       <c r="D60" s="1">
-        <v>0.32144865393638611</v>
+        <v>0.016771620139479637</v>
       </c>
       <c r="E60" s="1">
-        <v>0.13442450761795044</v>
+        <v>0.0075861215591430664</v>
       </c>
       <c r="F60" t="s">
         <v>13</v>
@@ -2205,13 +2205,13 @@
         <v>23</v>
       </c>
       <c r="H60" s="1">
-        <v>5.7976618409156799E-2</v>
+        <v>0.0019028219394385815</v>
       </c>
       <c r="I60" s="1">
-        <v>0.58492070436477661</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.031640417873859406</v>
+      </c>
+    </row>
+    <row r="61" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>9</v>
       </c>
@@ -2222,10 +2222,10 @@
         <v>18</v>
       </c>
       <c r="D61" s="1">
-        <v>0.3062191903591156</v>
+        <v>0.015586298890411854</v>
       </c>
       <c r="E61" s="1">
-        <v>0.12903633713722229</v>
+        <v>0.007919621653854847</v>
       </c>
       <c r="F61" t="s">
         <v>13</v>
@@ -2234,10 +2234,10 @@
         <v>23</v>
       </c>
       <c r="H61" s="1">
-        <v>5.3307969123125076E-2</v>
+        <v>6.3840445363894105e-05</v>
       </c>
       <c r="I61" s="1">
-        <v>0.55913043022155762</v>
+        <v>0.031108757480978966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>